<commit_message>
solve minor error in vocab
</commit_message>
<xml_diff>
--- a/templates/vocabulary_es_ca_gl.xlsx
+++ b/templates/vocabulary_es_ca_gl.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="n0rzbODzVndrwVNg9eNs9hsRCaaxK9LK3Wkv9sctb7I="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="tHRklnKNFIxv7Xhwek2TarYm4dtXspYIWmrE2AzTgPA="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="184">
   <si>
     <t>category</t>
   </si>
@@ -142,12 +142,6 @@
   </si>
   <si>
     <t>índia</t>
-  </si>
-  <si>
-    <t>inmigrante</t>
-  </si>
-  <si>
-    <t>inmigrant</t>
   </si>
   <si>
     <t>latino</t>
@@ -1411,17 +1405,21 @@
         <v>21</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1447,110 +1445,110 @@
       <c r="AF13" s="6"/>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8"/>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="8"/>
-      <c r="AE15" s="8"/>
-      <c r="AF15" s="8"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1579,112 +1577,112 @@
       <c r="AF16" s="6"/>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="6"/>
+      <c r="A17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="8"/>
       <c r="C17" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="6"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="6"/>
-      <c r="X17" s="6"/>
-      <c r="Y17" s="6"/>
-      <c r="Z17" s="6"/>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="6"/>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="6"/>
-      <c r="AE17" s="6"/>
-      <c r="AF17" s="6"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="8"/>
+      <c r="AC17" s="8"/>
+      <c r="AD17" s="8"/>
+      <c r="AE17" s="8"/>
+      <c r="AF17" s="8"/>
     </row>
     <row r="18">
-      <c r="A18" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6" t="s">
+      <c r="A18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="D18" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="8"/>
-      <c r="AB18" s="8"/>
-      <c r="AC18" s="8"/>
-      <c r="AD18" s="8"/>
-      <c r="AE18" s="8"/>
-      <c r="AF18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6"/>
+      <c r="AE18" s="6"/>
+      <c r="AF18" s="6"/>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" s="6"/>
-      <c r="C19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H19" s="8"/>
+      <c r="C19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -1712,24 +1710,20 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="E20" s="6"/>
-      <c r="F20" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="I20" s="8"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1756,7 +1750,7 @@
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6" t="s">
@@ -1769,7 +1763,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="8"/>
+      <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1796,22 +1790,36 @@
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="C22" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="K22" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
@@ -1836,35 +1844,37 @@
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="G23" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="J23" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="10" t="s">
-        <v>79</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
@@ -1890,37 +1900,37 @@
     </row>
     <row r="24">
       <c r="A24" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J24" s="6" t="b">
         <v>0</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -1946,37 +1956,35 @@
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="J25" s="6" t="b">
-        <v>0</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="J25" s="6"/>
       <c r="K25" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
@@ -2002,35 +2010,37 @@
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="J26" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="J26" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="K26" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
@@ -2056,37 +2066,37 @@
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J27" s="6" t="b">
         <v>0</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -2112,37 +2122,37 @@
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J28" s="6" t="b">
         <v>0</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
@@ -2168,37 +2178,37 @@
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J29" s="6" t="b">
         <v>0</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
@@ -2224,37 +2234,37 @@
     </row>
     <row r="30">
       <c r="A30" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J30" s="6" t="b">
         <v>0</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
@@ -2280,37 +2290,37 @@
     </row>
     <row r="31">
       <c r="A31" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J31" s="6" t="b">
         <v>0</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
@@ -2336,37 +2346,37 @@
     </row>
     <row r="32">
       <c r="A32" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>78</v>
+        <v>138</v>
       </c>
       <c r="J32" s="6" t="b">
         <v>0</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
@@ -2392,37 +2402,37 @@
     </row>
     <row r="33">
       <c r="A33" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G33" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I33" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>140</v>
       </c>
       <c r="J33" s="6" t="b">
         <v>0</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
@@ -2448,37 +2458,35 @@
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="J34" s="6" t="b">
-        <v>0</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="J34" s="6"/>
       <c r="K34" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
@@ -2504,35 +2512,37 @@
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="J35" s="6"/>
+        <v>138</v>
+      </c>
+      <c r="J35" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="K35" s="10" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
@@ -2558,37 +2568,37 @@
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J36" s="6" t="b">
         <v>0</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
@@ -2614,37 +2624,35 @@
     </row>
     <row r="37">
       <c r="A37" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="J37" s="6" t="b">
-        <v>0</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="J37" s="6"/>
       <c r="K37" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
@@ -2670,35 +2678,37 @@
     </row>
     <row r="38">
       <c r="A38" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="J38" s="6"/>
+        <v>138</v>
+      </c>
+      <c r="J38" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="K38" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
@@ -2724,37 +2734,37 @@
     </row>
     <row r="39">
       <c r="A39" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J39" s="6" t="b">
         <v>0</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
@@ -2780,37 +2790,37 @@
     </row>
     <row r="40">
       <c r="A40" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J40" s="6" t="b">
         <v>0</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
@@ -2836,38 +2846,24 @@
     </row>
     <row r="41">
       <c r="A41" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>71</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="B41" s="6"/>
       <c r="C41" s="6" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="H41" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="I41" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="J41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K41" s="10" t="s">
-        <v>127</v>
-      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
@@ -2891,23 +2887,15 @@
       <c r="AF41" s="6"/>
     </row>
     <row r="42">
-      <c r="A42" s="6" t="s">
-        <v>184</v>
-      </c>
+      <c r="A42" s="6"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>185</v>
-      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
-      <c r="I42" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="I42" s="6"/>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
@@ -25100,61 +25088,27 @@
       <c r="AE694" s="6"/>
       <c r="AF694" s="6"/>
     </row>
-    <row r="695">
-      <c r="A695" s="6"/>
-      <c r="B695" s="6"/>
-      <c r="C695" s="6"/>
-      <c r="D695" s="6"/>
-      <c r="E695" s="6"/>
-      <c r="F695" s="6"/>
-      <c r="G695" s="6"/>
-      <c r="H695" s="6"/>
-      <c r="I695" s="6"/>
-      <c r="J695" s="6"/>
-      <c r="K695" s="6"/>
-      <c r="L695" s="6"/>
-      <c r="M695" s="6"/>
-      <c r="N695" s="6"/>
-      <c r="O695" s="6"/>
-      <c r="P695" s="6"/>
-      <c r="Q695" s="6"/>
-      <c r="R695" s="6"/>
-      <c r="S695" s="6"/>
-      <c r="T695" s="6"/>
-      <c r="U695" s="6"/>
-      <c r="V695" s="6"/>
-      <c r="W695" s="6"/>
-      <c r="X695" s="6"/>
-      <c r="Y695" s="6"/>
-      <c r="Z695" s="6"/>
-      <c r="AA695" s="6"/>
-      <c r="AB695" s="6"/>
-      <c r="AC695" s="6"/>
-      <c r="AD695" s="6"/>
-      <c r="AE695" s="6"/>
-      <c r="AF695" s="6"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="K23"/>
-    <hyperlink r:id="rId2" ref="K24"/>
-    <hyperlink r:id="rId3" ref="K25"/>
-    <hyperlink r:id="rId4" ref="K26"/>
-    <hyperlink r:id="rId5" ref="K27"/>
-    <hyperlink r:id="rId6" ref="K28"/>
-    <hyperlink r:id="rId7" ref="K29"/>
-    <hyperlink r:id="rId8" ref="K30"/>
-    <hyperlink r:id="rId9" ref="K31"/>
-    <hyperlink r:id="rId10" ref="K32"/>
-    <hyperlink r:id="rId11" ref="K33"/>
-    <hyperlink r:id="rId12" ref="K34"/>
-    <hyperlink r:id="rId13" ref="K35"/>
-    <hyperlink r:id="rId14" ref="K36"/>
-    <hyperlink r:id="rId15" ref="K37"/>
-    <hyperlink r:id="rId16" ref="K38"/>
-    <hyperlink r:id="rId17" ref="K39"/>
-    <hyperlink r:id="rId18" ref="K40"/>
-    <hyperlink r:id="rId19" ref="K41"/>
+    <hyperlink r:id="rId1" ref="K22"/>
+    <hyperlink r:id="rId2" ref="K23"/>
+    <hyperlink r:id="rId3" ref="K24"/>
+    <hyperlink r:id="rId4" ref="K25"/>
+    <hyperlink r:id="rId5" ref="K26"/>
+    <hyperlink r:id="rId6" ref="K27"/>
+    <hyperlink r:id="rId7" ref="K28"/>
+    <hyperlink r:id="rId8" ref="K29"/>
+    <hyperlink r:id="rId9" ref="K30"/>
+    <hyperlink r:id="rId10" ref="K31"/>
+    <hyperlink r:id="rId11" ref="K32"/>
+    <hyperlink r:id="rId12" ref="K33"/>
+    <hyperlink r:id="rId13" ref="K34"/>
+    <hyperlink r:id="rId14" ref="K35"/>
+    <hyperlink r:id="rId15" ref="K36"/>
+    <hyperlink r:id="rId16" ref="K37"/>
+    <hyperlink r:id="rId17" ref="K38"/>
+    <hyperlink r:id="rId18" ref="K39"/>
+    <hyperlink r:id="rId19" ref="K40"/>
   </hyperlinks>
   <drawing r:id="rId20"/>
 </worksheet>

</xml_diff>